<commit_message>
Update key_properties in ocean mapping
</commit_message>
<xml_diff>
--- a/mappings/ocean-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/ocean-cmip5-to-cmip6-mappings.xlsx
@@ -1,33 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-ocean/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460"/>
+    <workbookView xWindow="1560" yWindow="1980" windowWidth="28800" windowHeight="17460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="157">
   <si>
     <t>Ocean &gt; Advection</t>
   </si>
@@ -450,6 +445,54 @@
   </si>
   <si>
     <t>Time Stepping Framework &gt; Tracer Time Stepping</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.bathymetry.type</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.bathymetry.reference_dates</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.grid.discretisation.horizontal.scheme</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.grid.discretisation.horizontal.type</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.prognostic_variables</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.model_family</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.nonoceanic_waters.isolated_seas</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.nonoceanic_waters.river_mouth</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.seawater_properties.eos_type</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.seawater_properties.ocean_freezing_point</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.key_properties.seawater_properties.ocean_specific_heat</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.timestepping_framework.barotropic_momentum_scheme.barotropic_momentum</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.timestepping_framework.barotropic_solver_scheme.type</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.timestepping_framework.barotropic_solver_scheme.barotropic_solver</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.timestepping_framework.timestepping_attributes.time_step</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.timestepping_framework.timestepping_tracers_scheme.tracers</t>
   </si>
 </sst>
 </file>
@@ -662,8 +705,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1853,11 +1896,11 @@
   </sheetPr>
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="44.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="1" bestFit="1" customWidth="1"/>
@@ -1865,7 +1908,7 @@
     <col min="4" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="31" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>102</v>
       </c>
@@ -1876,7 +1919,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="20.5" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -1887,43 +1930,51 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="20.5" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C3" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.5" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="5"/>
-    </row>
-    <row r="5" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C4" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.5" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C5" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.5" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C6" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.5" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>137</v>
       </c>
@@ -1932,43 +1983,51 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="20.5" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C8" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20.5" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C9" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="20.5" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C10" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.5" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="5"/>
-    </row>
-    <row r="12" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C11" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20.5" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>137</v>
       </c>
@@ -1977,7 +2036,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="20.5" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>137</v>
       </c>
@@ -1986,7 +2045,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="20.5" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>137</v>
       </c>
@@ -1995,7 +2054,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="20.5" customHeight="1">
       <c r="A15" s="2" t="s">
         <v>137</v>
       </c>
@@ -2004,7 +2063,7 @@
       </c>
       <c r="C15" s="5"/>
     </row>
-    <row r="16" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="20.5" customHeight="1">
       <c r="A16" s="2" t="s">
         <v>137</v>
       </c>
@@ -2013,7 +2072,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="20.5" customHeight="1">
       <c r="A17" s="2" t="s">
         <v>137</v>
       </c>
@@ -2022,7 +2081,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="20.5" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>137</v>
       </c>
@@ -2031,7 +2090,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="20.5" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>137</v>
       </c>
@@ -2040,7 +2099,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="20.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>137</v>
       </c>
@@ -2049,7 +2108,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="20.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>137</v>
       </c>
@@ -2058,7 +2117,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="20.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>137</v>
       </c>
@@ -2067,7 +2126,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="20.5" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>137</v>
       </c>
@@ -2076,7 +2135,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="20.5" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>137</v>
       </c>
@@ -2085,25 +2144,29 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="20.5" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C25" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.5" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C26" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20.5" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>137</v>
       </c>
@@ -2112,16 +2175,18 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="20.5" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C28" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20.5" customHeight="1">
       <c r="A29" s="2" t="s">
         <v>137</v>
       </c>
@@ -2130,52 +2195,62 @@
       </c>
       <c r="C29" s="5"/>
     </row>
-    <row r="30" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="20.5" customHeight="1">
       <c r="A30" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C30" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="20.5" customHeight="1">
       <c r="A31" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C31" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="20.5" customHeight="1">
       <c r="A32" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C32" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="20.5" customHeight="1">
       <c r="A33" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C33" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.5" customHeight="1">
       <c r="A34" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C34" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.5" customHeight="1">
       <c r="A35" s="2" t="s">
         <v>137</v>
       </c>
@@ -2184,12 +2259,12 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="20.5" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="20.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2200,7 +2275,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
@@ -2211,7 +2286,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -2222,7 +2297,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
@@ -2233,7 +2308,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
@@ -2244,7 +2319,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="20.25" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>0</v>
       </c>
@@ -2255,12 +2330,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="20.25" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -2271,7 +2346,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="20.25" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -2282,7 +2357,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" ht="20.25" customHeight="1">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -2293,12 +2368,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:3" ht="20.25" customHeight="1">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>11</v>
       </c>
@@ -2309,7 +2384,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
@@ -2320,7 +2395,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>11</v>
       </c>
@@ -2331,7 +2406,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>11</v>
       </c>
@@ -2342,7 +2417,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>11</v>
       </c>
@@ -2351,7 +2426,7 @@
       </c>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>11</v>
       </c>
@@ -2360,7 +2435,7 @@
       </c>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>11</v>
       </c>
@@ -2369,12 +2444,12 @@
       </c>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>19</v>
       </c>
@@ -2385,7 +2460,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="20.25" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>19</v>
       </c>
@@ -2394,7 +2469,7 @@
       </c>
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="20.25" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>19</v>
       </c>
@@ -2405,7 +2480,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>19</v>
       </c>
@@ -2416,7 +2491,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>19</v>
       </c>
@@ -2427,12 +2502,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
     </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2518,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" ht="20.25" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>19</v>
       </c>
@@ -2454,7 +2529,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>19</v>
       </c>
@@ -2465,12 +2540,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
     </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>28</v>
       </c>
@@ -2481,7 +2556,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>28</v>
       </c>
@@ -2492,7 +2567,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="4" t="s">
         <v>28</v>
       </c>
@@ -2501,7 +2576,7 @@
       </c>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>28</v>
       </c>
@@ -2512,7 +2587,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>28</v>
       </c>
@@ -2523,12 +2598,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
     </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>28</v>
       </c>
@@ -2539,7 +2614,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>28</v>
       </c>
@@ -2548,7 +2623,7 @@
       </c>
       <c r="C73" s="5"/>
     </row>
-    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:3" ht="20.25" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>28</v>
       </c>
@@ -2559,7 +2634,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:3" ht="20.25" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>28</v>
       </c>
@@ -2570,7 +2645,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:3" ht="20.25" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>28</v>
       </c>
@@ -2581,12 +2656,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:3" ht="20.25" customHeight="1">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
     </row>
-    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:3" ht="20.25" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>28</v>
       </c>
@@ -2597,7 +2672,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>28</v>
       </c>
@@ -2608,7 +2683,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:3" ht="20.25" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>28</v>
       </c>
@@ -2619,7 +2694,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" ht="20.25" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>28</v>
       </c>
@@ -2630,12 +2705,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:3" ht="20.25" customHeight="1">
       <c r="A82" s="4"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" ht="20.25" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>36</v>
       </c>
@@ -2646,7 +2721,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" ht="20.25" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>36</v>
       </c>
@@ -2657,7 +2732,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" ht="20.25" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>36</v>
       </c>
@@ -2668,7 +2743,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" ht="20.25" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>36</v>
       </c>
@@ -2679,12 +2754,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" ht="20.25" customHeight="1">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:3" ht="20.25" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>41</v>
       </c>
@@ -2695,7 +2770,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" ht="20.25" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>41</v>
       </c>
@@ -2706,12 +2781,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" ht="20.25" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" ht="20.25" customHeight="1">
       <c r="A91" s="4" t="s">
         <v>44</v>
       </c>
@@ -2722,7 +2797,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" ht="20.25" customHeight="1">
       <c r="A92" s="4" t="s">
         <v>44</v>
       </c>
@@ -2731,7 +2806,7 @@
       </c>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" ht="20.25" customHeight="1">
       <c r="A93" s="4" t="s">
         <v>44</v>
       </c>
@@ -2742,7 +2817,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" ht="20.25" customHeight="1">
       <c r="A94" s="4" t="s">
         <v>44</v>
       </c>
@@ -2753,12 +2828,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" ht="20.25" customHeight="1">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" ht="20.25" customHeight="1">
       <c r="A96" s="4" t="s">
         <v>44</v>
       </c>
@@ -2769,7 +2844,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:3" ht="20.25" customHeight="1">
       <c r="A97" s="4" t="s">
         <v>44</v>
       </c>
@@ -2778,7 +2853,7 @@
       </c>
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:3" ht="20.25" customHeight="1">
       <c r="A98" s="4" t="s">
         <v>44</v>
       </c>
@@ -2789,7 +2864,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" ht="20.25" customHeight="1">
       <c r="A99" s="4" t="s">
         <v>44</v>
       </c>
@@ -2800,12 +2875,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" ht="20.25" customHeight="1">
       <c r="A100" s="4"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:3" ht="20.25" customHeight="1">
       <c r="A101" s="4" t="s">
         <v>52</v>
       </c>
@@ -2816,7 +2891,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:3" ht="20.25" customHeight="1">
       <c r="A102" s="4" t="s">
         <v>52</v>
       </c>
@@ -2827,12 +2902,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:3" ht="20.25" customHeight="1">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:3" ht="20.25" customHeight="1">
       <c r="A104" s="4" t="s">
         <v>52</v>
       </c>
@@ -2843,7 +2918,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" ht="20.25" customHeight="1">
       <c r="A105" s="4" t="s">
         <v>52</v>
       </c>
@@ -2860,5 +2935,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update mappings to v 0.8.0
</commit_message>
<xml_diff>
--- a/mappings/ocean-cmip5-to-cmip6-mappings.xlsx
+++ b/mappings/ocean-cmip5-to-cmip6-mappings.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26819"/>
   <workbookPr date1904="1" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/cmip6/cmip6-specializations-ocean/mappings/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1980" windowWidth="39800" windowHeight="23940"/>
+    <workbookView xWindow="-120" yWindow="320" windowWidth="21680" windowHeight="25340"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -317,9 +312,6 @@
     <t>cmip6.ocean.advection.lateral_tracers.flux_limiter</t>
   </si>
   <si>
-    <t>cmip6.ocean.advection.lateral_tracers.type</t>
-  </si>
-  <si>
     <t>cmip6.ocean.advection.momentum.scheme_name</t>
   </si>
   <si>
@@ -329,9 +321,6 @@
     <t>cmip6.ocean.advection.vertical_tracers.flux_limiter</t>
   </si>
   <si>
-    <t>cmip6.ocean.advection.vertical_tracers.type</t>
-  </si>
-  <si>
     <t>cmip6.ocean.boundary_forcing.momentum_flux_correction</t>
   </si>
   <si>
@@ -489,6 +478,12 @@
   </si>
   <si>
     <t>cmip6.ocean.timestepping_framework.tracers.scheme</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.advection.vertical_tracers.name</t>
+  </si>
+  <si>
+    <t>cmip6.ocean.advection.lateral_tracers.name</t>
   </si>
 </sst>
 </file>
@@ -701,8 +696,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1892,369 +1887,369 @@
   </sheetPr>
   <dimension ref="A1:C105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="44.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="54.33203125" style="1" customWidth="1"/>
     <col min="4" max="254" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" ht="31" customHeight="1">
       <c r="A1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="C3" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A11" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A12" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="5"/>
+    </row>
+    <row r="15" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="C34" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="5" t="s">
+    <row r="35" spans="1:3" ht="20.5" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C30" s="5"/>
-    </row>
-    <row r="31" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="20.5" customHeight="1">
       <c r="A36" s="2"/>
       <c r="B36" s="3"/>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="20.5" customHeight="1">
       <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2265,7 +2260,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="20.25" customHeight="1">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
@@ -2273,10 +2268,10 @@
         <v>2</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" customHeight="1">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -2284,10 +2279,10 @@
         <v>3</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="20.25" customHeight="1">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
@@ -2295,10 +2290,10 @@
         <v>4</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="20.25" customHeight="1">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
@@ -2306,10 +2301,10 @@
         <v>5</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="20.25" customHeight="1">
       <c r="A42" s="4" t="s">
         <v>0</v>
       </c>
@@ -2317,15 +2312,15 @@
         <v>6</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="20.25" customHeight="1">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
     </row>
-    <row r="44" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:3" ht="20.25" customHeight="1">
       <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
@@ -2336,7 +2331,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:3" ht="20.25" customHeight="1">
       <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
@@ -2347,7 +2342,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:3" ht="20.25" customHeight="1">
       <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
@@ -2355,15 +2350,15 @@
         <v>10</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="20.25" customHeight="1">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:3" ht="20.25" customHeight="1">
       <c r="A48" s="4" t="s">
         <v>11</v>
       </c>
@@ -2374,7 +2369,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:3" ht="20.25" customHeight="1">
       <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
@@ -2385,7 +2380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:3" ht="20.25" customHeight="1">
       <c r="A50" s="4" t="s">
         <v>11</v>
       </c>
@@ -2396,7 +2391,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:3" ht="20.25" customHeight="1">
       <c r="A51" s="4" t="s">
         <v>11</v>
       </c>
@@ -2407,7 +2402,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:3" ht="20.25" customHeight="1">
       <c r="A52" s="4" t="s">
         <v>11</v>
       </c>
@@ -2416,7 +2411,7 @@
       </c>
       <c r="C52" s="5"/>
     </row>
-    <row r="53" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:3" ht="20.25" customHeight="1">
       <c r="A53" s="4" t="s">
         <v>11</v>
       </c>
@@ -2425,7 +2420,7 @@
       </c>
       <c r="C53" s="5"/>
     </row>
-    <row r="54" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:3" ht="20.25" customHeight="1">
       <c r="A54" s="4" t="s">
         <v>11</v>
       </c>
@@ -2434,12 +2429,12 @@
       </c>
       <c r="C54" s="5"/>
     </row>
-    <row r="55" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:3" ht="20.25" customHeight="1">
       <c r="A55" s="4"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
     </row>
-    <row r="56" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:3" ht="20.25" customHeight="1">
       <c r="A56" s="4" t="s">
         <v>19</v>
       </c>
@@ -2450,7 +2445,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:3" ht="20.25" customHeight="1">
       <c r="A57" s="4" t="s">
         <v>19</v>
       </c>
@@ -2459,7 +2454,7 @@
       </c>
       <c r="C57" s="5"/>
     </row>
-    <row r="58" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:3" ht="20.25" customHeight="1">
       <c r="A58" s="4" t="s">
         <v>19</v>
       </c>
@@ -2470,7 +2465,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:3" ht="20.25" customHeight="1">
       <c r="A59" s="4" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +2476,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:3" ht="20.25" customHeight="1">
       <c r="A60" s="4" t="s">
         <v>19</v>
       </c>
@@ -2492,12 +2487,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:3" ht="20.25" customHeight="1">
       <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
     </row>
-    <row r="62" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:3" ht="20.25" customHeight="1">
       <c r="A62" s="4" t="s">
         <v>19</v>
       </c>
@@ -2508,7 +2503,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:3" ht="20.25" customHeight="1">
       <c r="A63" s="4" t="s">
         <v>19</v>
       </c>
@@ -2519,7 +2514,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:3" ht="20.25" customHeight="1">
       <c r="A64" s="4" t="s">
         <v>19</v>
       </c>
@@ -2530,12 +2525,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:3" ht="20.25" customHeight="1">
       <c r="A65" s="4"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
     </row>
-    <row r="66" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:3" ht="20.25" customHeight="1">
       <c r="A66" s="4" t="s">
         <v>28</v>
       </c>
@@ -2546,7 +2541,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:3" ht="20.25" customHeight="1">
       <c r="A67" s="4" t="s">
         <v>28</v>
       </c>
@@ -2557,7 +2552,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:3" ht="20.25" customHeight="1">
       <c r="A68" s="4" t="s">
         <v>28</v>
       </c>
@@ -2566,7 +2561,7 @@
       </c>
       <c r="C68" s="5"/>
     </row>
-    <row r="69" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:3" ht="20.25" customHeight="1">
       <c r="A69" s="4" t="s">
         <v>28</v>
       </c>
@@ -2577,7 +2572,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:3" ht="20.25" customHeight="1">
       <c r="A70" s="4" t="s">
         <v>28</v>
       </c>
@@ -2588,12 +2583,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:3" ht="20.25" customHeight="1">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
     </row>
-    <row r="72" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:3" ht="20.25" customHeight="1">
       <c r="A72" s="4" t="s">
         <v>28</v>
       </c>
@@ -2604,7 +2599,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:3" ht="20.25" customHeight="1">
       <c r="A73" s="4" t="s">
         <v>28</v>
       </c>
@@ -2613,7 +2608,7 @@
       </c>
       <c r="C73" s="5"/>
     </row>
-    <row r="74" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:3" ht="20.25" customHeight="1">
       <c r="A74" s="4" t="s">
         <v>28</v>
       </c>
@@ -2624,7 +2619,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:3" ht="20.25" customHeight="1">
       <c r="A75" s="4" t="s">
         <v>28</v>
       </c>
@@ -2635,7 +2630,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:3" ht="20.25" customHeight="1">
       <c r="A76" s="4" t="s">
         <v>28</v>
       </c>
@@ -2646,12 +2641,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:3" ht="20.25" customHeight="1">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
     </row>
-    <row r="78" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:3" ht="20.25" customHeight="1">
       <c r="A78" s="4" t="s">
         <v>28</v>
       </c>
@@ -2662,7 +2657,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:3" ht="20.25" customHeight="1">
       <c r="A79" s="4" t="s">
         <v>28</v>
       </c>
@@ -2673,7 +2668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:3" ht="20.25" customHeight="1">
       <c r="A80" s="4" t="s">
         <v>28</v>
       </c>
@@ -2684,7 +2679,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:3" ht="20.25" customHeight="1">
       <c r="A81" s="4" t="s">
         <v>28</v>
       </c>
@@ -2695,12 +2690,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:3" ht="20.25" customHeight="1">
       <c r="A82" s="4"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
     </row>
-    <row r="83" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:3" ht="20.25" customHeight="1">
       <c r="A83" s="4" t="s">
         <v>36</v>
       </c>
@@ -2711,7 +2706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:3" ht="20.25" customHeight="1">
       <c r="A84" s="4" t="s">
         <v>36</v>
       </c>
@@ -2722,7 +2717,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:3" ht="20.25" customHeight="1">
       <c r="A85" s="4" t="s">
         <v>36</v>
       </c>
@@ -2733,7 +2728,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:3" ht="20.25" customHeight="1">
       <c r="A86" s="4" t="s">
         <v>36</v>
       </c>
@@ -2744,12 +2739,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:3" ht="20.25" customHeight="1">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
     </row>
-    <row r="88" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:3" ht="20.25" customHeight="1">
       <c r="A88" s="4" t="s">
         <v>41</v>
       </c>
@@ -2760,7 +2755,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:3" ht="20.25" customHeight="1">
       <c r="A89" s="4" t="s">
         <v>41</v>
       </c>
@@ -2771,12 +2766,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:3" ht="20.25" customHeight="1">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
     </row>
-    <row r="91" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:3" ht="20.25" customHeight="1">
       <c r="A91" s="4" t="s">
         <v>44</v>
       </c>
@@ -2787,7 +2782,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:3" ht="20.25" customHeight="1">
       <c r="A92" s="4" t="s">
         <v>44</v>
       </c>
@@ -2796,7 +2791,7 @@
       </c>
       <c r="C92" s="5"/>
     </row>
-    <row r="93" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:3" ht="20.25" customHeight="1">
       <c r="A93" s="4" t="s">
         <v>44</v>
       </c>
@@ -2807,7 +2802,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:3" ht="20.25" customHeight="1">
       <c r="A94" s="4" t="s">
         <v>44</v>
       </c>
@@ -2818,12 +2813,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:3" ht="20.25" customHeight="1">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
     </row>
-    <row r="96" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:3" ht="20.25" customHeight="1">
       <c r="A96" s="4" t="s">
         <v>44</v>
       </c>
@@ -2834,7 +2829,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:3" ht="20.25" customHeight="1">
       <c r="A97" s="4" t="s">
         <v>44</v>
       </c>
@@ -2843,7 +2838,7 @@
       </c>
       <c r="C97" s="5"/>
     </row>
-    <row r="98" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:3" ht="20.25" customHeight="1">
       <c r="A98" s="4" t="s">
         <v>44</v>
       </c>
@@ -2854,7 +2849,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:3" ht="20.25" customHeight="1">
       <c r="A99" s="4" t="s">
         <v>44</v>
       </c>
@@ -2865,12 +2860,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:3" ht="20.25" customHeight="1">
       <c r="A100" s="4"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
     </row>
-    <row r="101" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:3" ht="20.25" customHeight="1">
       <c r="A101" s="4" t="s">
         <v>52</v>
       </c>
@@ -2881,7 +2876,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:3" ht="20.25" customHeight="1">
       <c r="A102" s="4" t="s">
         <v>52</v>
       </c>
@@ -2892,12 +2887,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:3" ht="20.25" customHeight="1">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
     </row>
-    <row r="104" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:3" ht="20.25" customHeight="1">
       <c r="A104" s="4" t="s">
         <v>52</v>
       </c>
@@ -2908,7 +2903,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:3" ht="20.25" customHeight="1">
       <c r="A105" s="4" t="s">
         <v>52</v>
       </c>
@@ -2925,5 +2920,10 @@
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>